<commit_message>
Add signaturies Capitalized name of the month Fix bug with non working last day of the month
</commit_message>
<xml_diff>
--- a/src/main/FilesRepository/test.xlsx
+++ b/src/main/FilesRepository/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://specificgroup-my.sharepoint.com/personal/roman_nesterenko_specific-group_com/Documents/Documents/Java/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://specificgroup-my.sharepoint.com/personal/roman_nesterenko_specific-group_com/Documents/Documents/Java/utils/apache-maven-3.8.7/bin/Report/src/main/FilesRepository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104817D1DA72145BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{980E0029-E99A-47DC-B151-9E110FBCAE30}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_F25DC773A252ABDACC104817D1DA72145BDE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{021AE5ED-D055-48FA-BCD3-984F94E276D5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Raman</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>46 1191274723</t>
-  </si>
-  <si>
-    <t>adad</t>
-  </si>
-  <si>
-    <t>ad</t>
   </si>
 </sst>
 </file>
@@ -119,10 +113,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -399,6 +389,7 @@
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -441,20 +432,6 @@
       </c>
       <c r="D3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>